<commit_message>
update model.xlsx and example about curves
</commit_message>
<xml_diff>
--- a/unlvr_data/docs/02_Model.xlsx
+++ b/unlvr_data/docs/02_Model.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UL\0001_Eg_Unilever\unlvr_data\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Docs Edwin\Dashboards\GMA-UL\v0\Github\0001_Eg_Unilever\unlvr_data\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Gral" sheetId="1" r:id="rId1"/>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="121">
   <si>
     <t>Investigation</t>
   </si>
@@ -306,9 +306,6 @@
   </si>
   <si>
     <t>TRACKING_DATA</t>
-  </si>
-  <si>
-    <t>GROSS_MARGIN*TURNOVER</t>
   </si>
   <si>
     <t>GRP_COST</t>
@@ -625,12 +622,47 @@
   <si>
     <t>[Slide8, DecisionTree?]</t>
   </si>
+  <si>
+    <t>Tableau Bidireccional</t>
+  </si>
+  <si>
+    <t>OPT2:</t>
+  </si>
+  <si>
+    <t>Por Usuario!</t>
+  </si>
+  <si>
+    <t>OP1:</t>
+  </si>
+  <si>
+    <t>--&gt;&gt;</t>
+  </si>
+  <si>
+    <t>--&gt; Por ahora va con Dummy data porque MSc no tiene claro el calculo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">--&gt; Idea General
+[‎24/‎02/‎2016 03:58 p.m.] Arizpe, Moises (MBMEX): 
+La idea general que estamos usando para graficar es esta:
+1. Creamos una tabla con los números del 1 al 40 en una columna llamada "X"
+2. Creamos un campo calculado llamado "Xajustado" que transforma la variable X al rango que queremos graficar. Por ejemplo si queremos graficar del 300 al 500, hacemos el cálculo Xajustado=X*5+300
+3. Creamos un campo calculado llamado "Y" que calcula la función que queremos utilizando Xajustado y cualquier otro parámetro
+Y ya con eso no necesitamos muchas tablas, sólo una con los números del 1 al 40 y el resto lo calculamos al vuelo
+(En la gráfica ponemos Xadj como columna y Y como filas)
+[‎24/‎02/‎2016 03:59 p.m.] Arizpe, Moises (MBMEX): 
+Creo que debí haber empezado por decir que queremos graficar Y=f(X, param1, param2,...)
+Ejemplo en: "unlvr_viz/ejemplo_curvas_exploracion"
+</t>
+  </si>
+  <si>
+    <t>GROSS_MARGIN*TURNOVER (Calculado arriba para UL pero no tenemos el de la competencia)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -718,8 +750,23 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -765,6 +812,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -898,7 +951,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -908,11 +961,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1002,15 +1051,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1060,16 +1130,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>736600</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>746125</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>34925</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>130175</xdr:rowOff>
+      <xdr:rowOff>3175</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1093,7 +1163,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1346200" y="1168400"/>
+          <a:off x="1676400" y="1041400"/>
           <a:ext cx="6118225" cy="866775"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1113,10 +1183,164 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>22225</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect b="47252"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2882900" y="3810001"/>
+          <a:ext cx="6118225" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3149600" y="4343400"/>
+          <a:ext cx="3022600" cy="12700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7191375" y="409575"/>
+          <a:ext cx="9239250" cy="714375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7477,7 +7701,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -14771,7 +14995,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -15036,10 +15260,10 @@
   <dimension ref="B3:P37"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="R36" sqref="R36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
@@ -15068,56 +15292,229 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C5" s="71" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="72"/>
+    </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
-      <c r="C6" s="5"/>
-      <c r="G6" s="4"/>
-      <c r="K6" s="4"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="74"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="74"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="76"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="M7" s="76"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="76"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="76"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="76"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="81"/>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="F13" s="2"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="O15" s="4"/>
-      <c r="P15" s="8"/>
+      <c r="P15" s="6"/>
     </row>
-    <row r="20" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="H20" s="4"/>
-      <c r="I20" s="8"/>
+    <row r="19" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D19" s="71" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="72"/>
     </row>
-    <row r="22" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G22" s="7"/>
+    <row r="20" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D20" s="73"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="74"/>
+      <c r="I20" s="75"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="76"/>
     </row>
-    <row r="23" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G23" s="7"/>
+    <row r="21" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D21" s="73"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="76"/>
     </row>
-    <row r="24" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G24" s="7"/>
+    <row r="22" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D22" s="73"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="77"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="76"/>
     </row>
-    <row r="25" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G25" s="7"/>
+    <row r="23" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D23" s="73"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="77"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="76"/>
     </row>
-    <row r="26" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G26" s="7"/>
+    <row r="24" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D24" s="73"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="77"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="76"/>
+    </row>
+    <row r="25" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D25" s="73"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="77"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="76"/>
+    </row>
+    <row r="26" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D26" s="73"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="77"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="76"/>
+    </row>
+    <row r="27" spans="4:13" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="D27" s="78"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="79" t="s">
+        <v>113</v>
+      </c>
+      <c r="G27" s="80"/>
+      <c r="H27" s="80"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="81"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="6"/>
-      <c r="F37" s="6"/>
+      <c r="B37" s="5"/>
+      <c r="F37" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15128,20 +15525,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K60"/>
+  <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" style="63" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.85546875" style="63" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="61" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" style="61" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
@@ -15150,968 +15547,1019 @@
     <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19"/>
-      <c r="B1" s="15" t="s">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17"/>
+      <c r="B1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="55" t="s">
+      <c r="E1" s="53" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16">
+      <c r="B2" s="14">
         <v>5</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="53" t="s">
+      <c r="E2" s="51" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="16">
+      <c r="B3" s="14">
         <v>5</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="53" t="s">
+      <c r="E3" s="51" t="s">
         <v>10</v>
       </c>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="91"/>
+      <c r="J3" s="91"/>
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="16">
+      <c r="B4" s="14">
         <v>5</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="53" t="s">
+      <c r="E4" s="84" t="s">
         <v>12</v>
       </c>
+      <c r="F4" s="92" t="s">
+        <v>117</v>
+      </c>
+      <c r="G4" s="91"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="91"/>
+      <c r="M4" s="91"/>
+      <c r="N4" s="91"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="15">
         <v>5</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="56" t="s">
-        <v>73</v>
-      </c>
+      <c r="E5" s="86" t="s">
+        <v>120</v>
+      </c>
+      <c r="F5" s="91"/>
+      <c r="G5" s="91"/>
+      <c r="H5" s="91"/>
+      <c r="I5" s="91"/>
+      <c r="J5" s="91"/>
+      <c r="K5" s="91"/>
+      <c r="L5" s="91"/>
+      <c r="M5" s="91"/>
+      <c r="N5" s="91"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="16">
         <v>6</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="57" t="s">
+      <c r="E6" s="55" t="s">
         <v>70</v>
       </c>
+      <c r="F6" s="91"/>
+      <c r="G6" s="91"/>
+      <c r="H6" s="91"/>
+      <c r="I6" s="91"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="91"/>
+      <c r="L6" s="91"/>
+      <c r="M6" s="91"/>
+      <c r="N6" s="91"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="16">
+      <c r="B7" s="14">
         <v>6</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="53" t="s">
+      <c r="E7" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="23" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B8" s="14">
         <v>6</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="53" t="s">
+      <c r="E8" s="51" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="16">
+      <c r="B9" s="14">
         <v>6</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="E9" s="53" t="s">
+      <c r="E9" s="51" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="16">
+      <c r="B10" s="14">
         <v>6</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="64"/>
-      <c r="E10" s="65"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="63"/>
       <c r="F10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="14">
+        <v>6</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" s="51" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="14">
+        <v>6</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="62"/>
+      <c r="E12" s="63"/>
+      <c r="F12" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="16">
+      <c r="B13" s="14">
         <v>6</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="51" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="15">
         <v>6</v>
       </c>
-      <c r="D11" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" s="53" t="s">
-        <v>67</v>
+      <c r="C14" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="31"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="89" t="s">
+        <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="16">
-        <v>6</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="64"/>
-      <c r="E12" s="65"/>
-      <c r="F12" t="s">
-        <v>77</v>
+      <c r="B15" s="19">
+        <v>7</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="57" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="16">
-        <v>6</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="53" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="17">
-        <v>6</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="34"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="21">
-        <v>7</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="58" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="59" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="18">
+      <c r="B16" s="16">
         <v>8</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="57" t="s">
+      <c r="E16" s="55" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="16">
+      <c r="B17" s="14">
         <v>8</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="53" t="s">
+      <c r="E17" s="51" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="16">
+      <c r="B18" s="14">
         <v>8</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D18" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="E18" s="53" t="s">
+      <c r="E18" s="51" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B19" s="16">
+      <c r="B19" s="14">
         <v>8</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="53" t="s">
-        <v>74</v>
+      <c r="E19" s="51" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="17">
+      <c r="B20" s="15">
         <v>8</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="56" t="s">
+      <c r="E20" s="54" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B21" s="16">
         <v>9</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="66"/>
-      <c r="E21" s="67"/>
-      <c r="F21" s="53" t="s">
-        <v>78</v>
+      <c r="D21" s="64"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="51" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="16">
+      <c r="B22" s="14">
         <v>9</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="66"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="53" t="s">
-        <v>79</v>
+      <c r="D22" s="64"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="51" t="s">
+        <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="23" t="s">
+    <row r="23" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="D23" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="57" t="s">
+      <c r="E23" s="55" t="s">
         <v>70</v>
       </c>
+      <c r="F23" s="90" t="s">
+        <v>119</v>
+      </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="27" t="s">
+    <row r="24" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="25" t="s">
+      <c r="D24" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="53" t="s">
+      <c r="E24" s="51" t="s">
         <v>23</v>
       </c>
+      <c r="F24" s="90"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
+    <row r="25" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="C25" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="25" t="s">
+      <c r="D25" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E25" s="53" t="s">
+      <c r="E25" s="51" t="s">
         <v>23</v>
       </c>
+      <c r="F25" s="90"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
+    <row r="26" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="25" t="s">
+      <c r="D26" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="E26" s="53" t="s">
+      <c r="E26" s="51" t="s">
         <v>31</v>
       </c>
+      <c r="F26" s="90"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="27" t="s">
+    <row r="27" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="25" t="s">
+      <c r="D27" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="E27" s="53" t="s">
-        <v>75</v>
-      </c>
+      <c r="E27" s="51" t="s">
+        <v>74</v>
+      </c>
+      <c r="F27" s="90"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="24" t="s">
+    <row r="28" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="28" t="s">
+      <c r="D28" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="E28" s="56" t="s">
+      <c r="E28" s="54" t="s">
         <v>68</v>
       </c>
+      <c r="F28" s="90"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="23" t="s">
+    <row r="29" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="18">
+      <c r="B29" s="16">
         <v>14</v>
       </c>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="D29" s="44"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="73"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="90"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
+    <row r="30" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B30" s="18">
+      <c r="B30" s="16">
         <v>15.16</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="D30" s="29"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="73"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="90"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="27" t="s">
+    <row r="31" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="16">
+      <c r="B31" s="14">
         <v>15.16</v>
       </c>
-      <c r="C31" s="25" t="s">
+      <c r="C31" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="31"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="73"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="90"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="27" t="s">
+    <row r="32" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="16">
+      <c r="B32" s="14">
         <v>15.16</v>
       </c>
-      <c r="C32" s="25" t="s">
+      <c r="C32" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="74"/>
-      <c r="E32" s="75"/>
-      <c r="F32" s="73"/>
+      <c r="D32" s="87"/>
+      <c r="E32" s="88"/>
+      <c r="F32" s="90"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="27" t="s">
+    <row r="33" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="16">
+      <c r="B33" s="14">
         <v>15.16</v>
       </c>
-      <c r="C33" s="25" t="s">
+      <c r="C33" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="31"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="73"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="90"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="27" t="s">
+    <row r="34" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B34" s="16">
+      <c r="B34" s="14">
         <v>15.16</v>
       </c>
-      <c r="C34" s="25" t="s">
+      <c r="C34" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="31"/>
-      <c r="E34" s="32"/>
-      <c r="F34" s="73"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="90"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="27" t="s">
+    <row r="35" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="16">
+      <c r="B35" s="14">
         <v>15.16</v>
       </c>
-      <c r="C35" s="25" t="s">
+      <c r="C35" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D35" s="31"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="73"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="90"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C36" s="37" t="s">
+      <c r="C36" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="D36" s="26" t="s">
+      <c r="D36" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="E36" s="57" t="s">
+      <c r="E36" s="55" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="38" t="s">
+      <c r="A37" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="39" t="s">
+      <c r="C37" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="25" t="s">
+      <c r="D37" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E37" s="53" t="s">
+      <c r="E37" s="51" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="38" t="s">
+      <c r="A38" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C38" s="39" t="s">
+      <c r="C38" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="D38" s="25" t="s">
+      <c r="D38" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E38" s="53" t="s">
+      <c r="E38" s="51" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="38" t="s">
+      <c r="A39" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="16" t="s">
+      <c r="B39" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="39" t="s">
+      <c r="C39" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="D39" s="25"/>
-      <c r="E39" s="53"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="51"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="38" t="s">
+      <c r="A40" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B40" s="16" t="s">
+      <c r="B40" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C40" s="39" t="s">
+      <c r="C40" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="D40" s="25" t="s">
+      <c r="D40" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E40" s="53" t="s">
+      <c r="E40" s="51" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="38" t="s">
+      <c r="A41" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B41" s="16" t="s">
+      <c r="B41" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C41" s="39" t="s">
+      <c r="C41" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="D41" s="25" t="s">
+      <c r="D41" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="E41" s="53" t="s">
+      <c r="E41" s="51" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="38" t="s">
+      <c r="A42" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B42" s="16" t="s">
+      <c r="B42" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="39" t="s">
+      <c r="C42" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="D42" s="25" t="s">
+      <c r="D42" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E42" s="53" t="s">
+      <c r="E42" s="51" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="38" t="s">
+      <c r="A43" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B43" s="16" t="s">
+      <c r="B43" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C43" s="39" t="s">
+      <c r="C43" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="D43" s="25" t="s">
+      <c r="D43" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="E43" s="53" t="s">
-        <v>74</v>
+      <c r="E43" s="51" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="38" t="s">
+      <c r="A44" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C44" s="39" t="s">
+      <c r="C44" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="D44" s="42" t="s">
+      <c r="D44" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="E44" s="60" t="s">
+      <c r="E44" s="58" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="38" t="s">
+      <c r="A45" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="16" t="s">
+      <c r="B45" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="39" t="s">
+      <c r="C45" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D45" s="25"/>
-      <c r="E45" s="53"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="51"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="38" t="s">
+      <c r="A46" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B46" s="16" t="s">
+      <c r="B46" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C46" s="39" t="s">
+      <c r="C46" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="D46" s="42" t="s">
+      <c r="D46" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="E46" s="60" t="s">
+      <c r="E46" s="58" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="40" t="s">
+      <c r="A47" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C47" s="41" t="s">
+      <c r="C47" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="D47" s="28"/>
-      <c r="E47" s="56"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="54"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="36" t="s">
+      <c r="A48" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="B48" s="18" t="s">
+      <c r="B48" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="C48" s="43" t="s">
+      <c r="C48" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="57"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="55"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="38" t="s">
+      <c r="A49" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B49" s="16" t="s">
+      <c r="B49" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C49" s="47" t="s">
+      <c r="C49" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="D49" s="25" t="s">
+      <c r="D49" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="E49" s="53" t="s">
+      <c r="E49" s="51" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="38" t="s">
+      <c r="A50" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B50" s="16" t="s">
+      <c r="B50" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C50" s="47" t="s">
+      <c r="C50" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="D50" s="25" t="s">
+      <c r="D50" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E50" s="53" t="s">
+      <c r="E50" s="51" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="38" t="s">
+      <c r="A51" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B51" s="16" t="s">
+      <c r="B51" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C51" s="47" t="s">
+      <c r="C51" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="D51" s="25"/>
-      <c r="E51" s="53"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="51"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="38" t="s">
+      <c r="A52" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B52" s="16" t="s">
+      <c r="B52" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C52" s="47" t="s">
+      <c r="C52" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="D52" s="25"/>
-      <c r="E52" s="53"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="51"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="38" t="s">
+      <c r="A53" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B53" s="16" t="s">
+      <c r="B53" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C53" s="47" t="s">
+      <c r="C53" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="D53" s="25"/>
-      <c r="E53" s="53"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="51"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="38" t="s">
+      <c r="A54" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="16" t="s">
+      <c r="B54" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C54" s="47" t="s">
+      <c r="C54" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="D54" s="61"/>
-      <c r="E54" s="62"/>
-      <c r="F54" s="46"/>
-      <c r="G54" s="35"/>
-      <c r="H54" s="35"/>
-      <c r="I54" s="35"/>
-      <c r="J54" s="35"/>
-      <c r="K54" s="35"/>
+      <c r="D54" s="59"/>
+      <c r="E54" s="60"/>
+      <c r="F54" s="44"/>
+      <c r="G54" s="33"/>
+      <c r="H54" s="33"/>
+      <c r="I54" s="33"/>
+      <c r="J54" s="33"/>
+      <c r="K54" s="33"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="38" t="s">
+      <c r="A55" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B55" s="16" t="s">
+      <c r="B55" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C55" s="47" t="s">
+      <c r="C55" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="D55" s="25"/>
-      <c r="E55" s="53"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="51"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="40" t="s">
+      <c r="A56" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B56" s="17" t="s">
+      <c r="B56" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C56" s="48" t="s">
+      <c r="C56" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="D56" s="28"/>
-      <c r="E56" s="56"/>
+      <c r="D56" s="26"/>
+      <c r="E56" s="54"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="49" t="s">
+      <c r="A57" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="18">
+      <c r="B57" s="16">
         <v>4</v>
       </c>
-      <c r="C57" s="43" t="s">
+      <c r="C57" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="D57" s="26"/>
-      <c r="E57" s="57"/>
+      <c r="D57" s="24"/>
+      <c r="E57" s="55"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="50" t="s">
+      <c r="A58" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="B58" s="16">
+      <c r="B58" s="14">
         <v>4</v>
       </c>
-      <c r="C58" s="47" t="s">
+      <c r="C58" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="D58" s="25"/>
-      <c r="E58" s="53"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="51"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="50" t="s">
+      <c r="A59" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="B59" s="16">
+      <c r="B59" s="14">
         <v>4</v>
       </c>
-      <c r="C59" s="52" t="s">
+      <c r="C59" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="D59" s="25" t="s">
+      <c r="D59" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E59" s="53" t="s">
+      <c r="E59" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="F59" s="42" t="s">
+      <c r="F59" s="40" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="51" t="s">
+      <c r="A60" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="B60" s="17">
+      <c r="B60" s="15">
         <v>4</v>
       </c>
-      <c r="C60" s="12" t="s">
+      <c r="C60" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="D60" s="28" t="s">
+      <c r="D60" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="E60" s="56" t="s">
+      <c r="E60" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="F60" s="42" t="s">
+      <c r="F60" s="40" t="s">
         <v>65</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="F29:F35"/>
     <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F23:F35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -16123,9 +16571,9 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="72"/>
+    <col min="1" max="16384" width="9.140625" style="70"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16142,7 +16590,7 @@
       <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
   </cols>
@@ -16156,9 +16604,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16168,243 +16616,243 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="68"/>
-    <col min="2" max="2" width="3.7109375" style="70" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="66"/>
+    <col min="2" max="2" width="3.7109375" style="68" customWidth="1"/>
     <col min="4" max="4" width="45.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
-        <v>84</v>
-      </c>
-      <c r="B1" s="70" t="s">
-        <v>80</v>
+      <c r="A1" s="66" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="68" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="68" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="B2" s="71"/>
-      <c r="C2" s="68" t="s">
+    <row r="2" spans="1:8" s="66" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="B2" s="69"/>
+      <c r="C2" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="66" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="66" t="s">
+        <v>104</v>
+      </c>
+      <c r="H2" s="66" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="66" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="B3" s="69"/>
+      <c r="C3" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="68" t="s">
+      <c r="D3" s="66" t="s">
         <v>101</v>
       </c>
-      <c r="E2" s="68" t="s">
-        <v>105</v>
-      </c>
-      <c r="H2" s="68" t="s">
-        <v>107</v>
+      <c r="E3" s="66" t="s">
+        <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="68" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="B3" s="71"/>
-      <c r="C3" s="68" t="s">
+    <row r="4" spans="1:8" s="66" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="B4" s="69"/>
+      <c r="C4" s="66" t="s">
         <v>99</v>
       </c>
-      <c r="D3" s="68" t="s">
+      <c r="D4" s="66" t="s">
         <v>102</v>
-      </c>
-      <c r="E3" s="68" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="68" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="B4" s="71"/>
-      <c r="C4" s="68" t="s">
-        <v>100</v>
-      </c>
-      <c r="D4" s="68" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="68" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" s="70" t="s">
-        <v>81</v>
+      <c r="A5" s="66" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="68" t="s">
+        <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="68" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="B6" s="71"/>
-      <c r="C6" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="E6" s="68" t="s">
-        <v>106</v>
-      </c>
-      <c r="H6" s="68" t="s">
+    <row r="6" spans="1:8" s="66" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="B6" s="69"/>
+      <c r="C6" s="66" t="s">
         <v>108</v>
       </c>
+      <c r="E6" s="66" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6" s="66" t="s">
+        <v>107</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" s="68" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="B7" s="71"/>
-      <c r="C7" s="68" t="s">
+    <row r="7" spans="1:8" s="66" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="B7" s="69"/>
+      <c r="C7" s="66" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="66" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="66" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="B8" s="69"/>
+      <c r="C8" s="66" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="68" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="68" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="B8" s="71"/>
-      <c r="C8" s="68" t="s">
-        <v>100</v>
-      </c>
-      <c r="E8" s="68" t="s">
-        <v>106</v>
+      <c r="E8" s="66" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="68" t="s">
-        <v>84</v>
-      </c>
-      <c r="B9" s="70" t="s">
-        <v>82</v>
+      <c r="A9" s="66" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="68" t="s">
+        <v>81</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="68" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="B10" s="71"/>
-      <c r="C10" s="68" t="s">
-        <v>109</v>
-      </c>
-      <c r="E10" s="68" t="s">
-        <v>106</v>
-      </c>
-      <c r="H10" s="68" t="s">
-        <v>113</v>
+    <row r="10" spans="1:8" s="66" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="B10" s="69"/>
+      <c r="C10" s="66" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" s="66" t="s">
+        <v>105</v>
+      </c>
+      <c r="H10" s="66" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="68" t="s">
-        <v>84</v>
-      </c>
-      <c r="B12" s="70" t="s">
+      <c r="A12" s="66" t="s">
         <v>83</v>
       </c>
+      <c r="B12" s="68" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="13" spans="1:8" s="68" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="B13" s="71"/>
-      <c r="C13" s="68" t="s">
-        <v>100</v>
-      </c>
-      <c r="D13" s="68" t="s">
+    <row r="13" spans="1:8" s="66" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="B13" s="69"/>
+      <c r="C13" s="66" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" s="66" t="s">
+        <v>110</v>
+      </c>
+      <c r="E13" s="66" t="s">
+        <v>105</v>
+      </c>
+      <c r="H13" s="66" t="s">
         <v>111</v>
       </c>
-      <c r="E13" s="68" t="s">
-        <v>106</v>
-      </c>
-      <c r="H13" s="68" t="s">
-        <v>112</v>
-      </c>
     </row>
-    <row r="14" spans="1:8" s="68" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="B14" s="71"/>
-      <c r="C14" s="68" t="s">
+    <row r="14" spans="1:8" s="66" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="B14" s="69"/>
+      <c r="C14" s="66" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="66" t="s">
         <v>109</v>
-      </c>
-      <c r="D14" s="68" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="68" t="s">
+      <c r="A15" s="66" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="68" t="s">
         <v>85</v>
-      </c>
-      <c r="B15" s="70" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="68" t="s">
-        <v>85</v>
-      </c>
-      <c r="B16" s="70" t="s">
-        <v>89</v>
-      </c>
-      <c r="D16" s="69"/>
+      <c r="A16" s="66" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="68" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="67"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="68" t="s">
-        <v>85</v>
-      </c>
-      <c r="B17" s="70" t="s">
-        <v>90</v>
-      </c>
-      <c r="D17" s="69"/>
+      <c r="A17" s="66" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="68" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="67"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="68" t="s">
-        <v>85</v>
-      </c>
-      <c r="B18" s="70" t="s">
-        <v>91</v>
-      </c>
-      <c r="D18" s="69"/>
+      <c r="A18" s="66" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="67"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="68" t="s">
-        <v>85</v>
-      </c>
-      <c r="B19" s="70" t="s">
-        <v>88</v>
-      </c>
-      <c r="D19" s="69"/>
+      <c r="A19" s="66" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="68" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="67"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="68" t="s">
-        <v>85</v>
-      </c>
-      <c r="B20" s="70" t="s">
-        <v>87</v>
-      </c>
-      <c r="D20" s="69"/>
+      <c r="A20" s="66" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="67"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="68" t="s">
+      <c r="A21" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" s="68" t="s">
         <v>92</v>
       </c>
-      <c r="B21" s="70" t="s">
-        <v>93</v>
-      </c>
-      <c r="D21" s="69"/>
+      <c r="D21" s="67"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="68" t="s">
-        <v>92</v>
-      </c>
-      <c r="B22" s="70" t="s">
-        <v>94</v>
+      <c r="A22" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" s="68" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="68" t="s">
-        <v>92</v>
-      </c>
-      <c r="B23" s="70" t="s">
-        <v>95</v>
+      <c r="A23" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="68" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="68" t="s">
-        <v>92</v>
-      </c>
-      <c r="B24" s="70" t="s">
-        <v>96</v>
+      <c r="A24" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="68" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="68" t="s">
-        <v>92</v>
-      </c>
-      <c r="B25" s="70" t="s">
-        <v>97</v>
+      <c r="A25" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" s="68" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>